<commit_message>
#1 Missile supprt more than 1 frame
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -74,11 +74,43 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>xxx</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>xxx</t>
+    <t>darkwheel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑暗轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑龙波</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragonball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FrameCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FrameTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每帧的时间</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -763,14 +795,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E6" totalsRowShown="0">
-  <autoFilter ref="A3:E6"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G8" totalsRowShown="0">
+  <autoFilter ref="A3:G8"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="TypeName"/>
     <tableColumn id="3" name="Name"/>
     <tableColumn id="4" name="Speed"/>
     <tableColumn id="5" name="Image"/>
+    <tableColumn id="6" name="FrameCount"/>
+    <tableColumn id="7" name="FrameTime"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1063,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1074,7 +1108,7 @@
     <col min="2" max="2" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1090,8 +1124,14 @@
       <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1105,10 +1145,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1124,8 +1170,14 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1141,13 +1193,19 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1156,10 +1214,16 @@
         <v>3</v>
       </c>
       <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1173,7 +1237,59 @@
         <v>7</v>
       </c>
       <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
         <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4 add some data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Missile" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -30,87 +30,119 @@
     <t>Image</t>
   </si>
   <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>速度</t>
+  </si>
+  <si>
+    <t>弓箭</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>类型名</t>
+  </si>
+  <si>
+    <t>序列</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>路径</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxx</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkwheel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑暗轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑龙波</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragonball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FrameCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FrameTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每帧的时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>arrow</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>速度</t>
-  </si>
-  <si>
-    <t>弓箭</t>
-  </si>
-  <si>
-    <t>TypeName</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>类型名</t>
-  </si>
-  <si>
-    <t>序列</t>
-  </si>
-  <si>
-    <t>名字</t>
-  </si>
-  <si>
-    <t>路径</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>null</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>默认图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxx</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkwheel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑暗轮</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑龙波</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dragonball</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FrameCount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FrameTime</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每帧的时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrowred</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrowlight</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluepea</t>
+  </si>
+  <si>
+    <t>greenpea</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝色豆子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿色豆子</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -795,8 +827,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G8" totalsRowShown="0">
-  <autoFilter ref="A3:G8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G12" totalsRowShown="0">
+  <autoFilter ref="A3:G12"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="TypeName"/>
@@ -1097,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1110,48 +1142,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1159,22 +1191,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1182,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1205,10 +1237,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1228,10 +1260,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -1251,10 +1283,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1274,10 +1306,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1289,7 +1321,99 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload missile image & config #4
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>xxx</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -143,6 +139,133 @@
   </si>
   <si>
     <t>绿色豆子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bullet</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>electball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>电球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>firearrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>花粉</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>flowerline</t>
+  </si>
+  <si>
+    <t>fireball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>holybolt</t>
+  </si>
+  <si>
+    <t>圣光弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>iceball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>laser2</t>
+  </si>
+  <si>
+    <t>激光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>leafarrow</t>
+  </si>
+  <si>
+    <t>叶子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>purplebubble</t>
+  </si>
+  <si>
+    <t>紫色泡泡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>purpleline</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫色线条</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>purplewave</t>
+  </si>
+  <si>
+    <t>紫色光圈</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rocket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>长矛</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterbolt</t>
+  </si>
+  <si>
+    <t>水箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterball</t>
+  </si>
+  <si>
+    <t>水球</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -827,8 +950,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G12" totalsRowShown="0">
-  <autoFilter ref="A3:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G28" totalsRowShown="0">
+  <autoFilter ref="A3:G28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="TypeName"/>
@@ -1129,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1157,10 +1280,10 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1177,13 +1300,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1203,10 +1326,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1237,13 +1360,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1260,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1283,10 +1406,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1306,10 +1429,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1329,10 +1452,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1352,10 +1475,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1375,10 +1498,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1398,10 +1521,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -1413,6 +1536,374 @@
         <v>1</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>110</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>130</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>140</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>150</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>160</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>170</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>180</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>190</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>200</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>210</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>220</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>230</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>240</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#4 remake image for effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -266,6 +266,46 @@
   </si>
   <si>
     <t>水球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>electhit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>电击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风刃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>windsharp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkfire</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗焰</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>firewall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterwall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火墙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水墙</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -950,8 +990,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G28" totalsRowShown="0">
-  <autoFilter ref="A3:G28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G33" totalsRowShown="0">
+  <autoFilter ref="A3:G33"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="TypeName"/>
@@ -1252,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1907,6 +1947,121 @@
         <v>1</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>250</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>260</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>270</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>280</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>290</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
compelete missile image effect #4
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -1294,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1688,10 +1688,10 @@
         <v>130</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
@@ -1757,10 +1757,10 @@
         <v>160</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -1780,10 +1780,10 @@
         <v>170</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -1803,10 +1803,10 @@
         <v>180</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1872,10 +1872,10 @@
         <v>210</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix new card firewall and laser
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>Id</t>
   </si>
@@ -293,19 +293,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>waterwall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火墙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水墙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>laser</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激光黄</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>firewall</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>waterwall</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>火墙</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水墙</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -990,8 +998,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G33" totalsRowShown="0">
-  <autoFilter ref="A3:G33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G34" totalsRowShown="0">
+  <autoFilter ref="A3:G34"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="TypeName"/>
@@ -1292,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2021,10 +2029,10 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -2044,10 +2052,10 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2059,6 +2067,29 @@
         <v>1</v>
       </c>
       <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>300</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rearange the path of minigame image
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -986,6 +986,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1021,7 +1089,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1302,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1311,7 +1379,7 @@
     <col min="2" max="2" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
optimise 2 summon hit skill effects
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
   <si>
     <t>Id</t>
   </si>
@@ -394,6 +394,14 @@
   </si>
   <si>
     <t>purplestarflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrowfast</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>弓箭快</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1078,10 +1086,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H39" totalsRowShown="0">
-  <autoFilter ref="A3:H39"/>
-  <sortState ref="A4:H35">
-    <sortCondition ref="A3:A35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H40" totalsRowShown="0">
+  <autoFilter ref="A3:H40"/>
+  <sortState ref="A4:H36">
+    <sortCondition ref="A3:A36"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
@@ -1418,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1566,25 +1574,25 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -1592,25 +1600,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -1618,25 +1626,25 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
@@ -1644,19 +1652,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1670,19 +1678,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1696,19 +1704,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1722,19 +1730,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1748,25 +1756,25 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -1774,25 +1782,25 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -1800,19 +1808,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1826,25 +1834,25 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
@@ -1852,22 +1860,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -1878,25 +1886,25 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
@@ -1904,25 +1912,25 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
@@ -1930,22 +1938,22 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>2</v>
@@ -1956,25 +1964,25 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21">
         <v>4</v>
       </c>
       <c r="F21">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
         <v>2</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
@@ -1982,22 +1990,22 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>3</v>
@@ -2008,25 +2016,25 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
@@ -2034,25 +2042,25 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E24">
         <v>4</v>
       </c>
       <c r="F24">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
@@ -2060,25 +2068,25 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
@@ -2086,25 +2094,25 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
@@ -2112,25 +2120,25 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
@@ -2138,25 +2146,25 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E28">
         <v>4</v>
       </c>
       <c r="F28">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
@@ -2164,25 +2172,25 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
@@ -2190,25 +2198,25 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F30">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
@@ -2216,22 +2224,22 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -2242,25 +2250,25 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
@@ -2268,19 +2276,19 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2294,25 +2302,25 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
@@ -2320,22 +2328,22 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2346,19 +2354,19 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -2372,22 +2380,22 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -2398,25 +2406,25 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E38">
         <v>5</v>
       </c>
       <c r="F38">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="G38">
         <v>2</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
@@ -2424,24 +2432,50 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F39">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="G39">
         <v>2</v>
       </c>
       <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>360</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
balance the weapon and skills
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Missile.xlsx
+++ b/ConfigData/Xlsx/Missile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="105">
   <si>
     <t>Id</t>
   </si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t>弓箭快</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowsplash</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1074,6 +1086,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1086,8 +1166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H40" totalsRowShown="0">
-  <autoFilter ref="A3:H40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H41" totalsRowShown="0">
+  <autoFilter ref="A3:H41"/>
   <sortState ref="A4:H36">
     <sortCondition ref="A3:A36"/>
   </sortState>
@@ -1113,7 +1193,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1426,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1437,6 +1517,7 @@
     <col min="1" max="1" width="5.625" customWidth="1"/>
     <col min="2" max="2" width="10.75" customWidth="1"/>
     <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="5" max="8" width="5.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.15">
@@ -2477,6 +2558,32 @@
       </c>
       <c r="H40">
         <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>370</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>